<commit_message>
updated latitudes and longitudes, added Foronda village
</commit_message>
<xml_diff>
--- a/regresiones_era5_observados_conalturas/sesgos_tmax_tmin.xlsx
+++ b/regresiones_era5_observados_conalturas/sesgos_tmax_tmin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tmin</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t xml:space="preserve">Zumarraga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foronda-Txokiza</t>
   </si>
   <si>
     <t xml:space="preserve">ERA5Land height</t>
@@ -321,7 +327,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +350,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF099"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6B26B"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -395,7 +407,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,6 +465,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,7 +526,7 @@
       <rgbColor rgb="FFA4C2F4"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFF6B26B"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -537,10 +553,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1141,6 +1157,46 @@
       </c>
       <c r="S11" s="13"/>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>16.99</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>35</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>31.21</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>16.82</v>
+      </c>
+      <c r="I12" s="11" t="n">
+        <f aca="false">D12-H12</f>
+        <v>0.169999999999998</v>
+      </c>
+      <c r="J12" s="8" t="n">
+        <v>35</v>
+      </c>
+      <c r="K12" s="9" t="n">
+        <v>31.04</v>
+      </c>
+      <c r="L12" s="11" t="n">
+        <f aca="false">F12-K12</f>
+        <v>0.170000000000002</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -1148,10 +1204,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,7 +1217,7 @@
       <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15" t="n">
+      <c r="C15" s="16" t="n">
         <v>361.32</v>
       </c>
       <c r="D15" s="1" t="n">
@@ -1175,7 +1231,7 @@
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15" t="n">
+      <c r="C16" s="16" t="n">
         <v>441.31</v>
       </c>
       <c r="D16" s="1" t="n">
@@ -1189,7 +1245,7 @@
       <c r="B17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="16" t="n">
         <v>344.83</v>
       </c>
       <c r="D17" s="1" t="n">
@@ -1203,7 +1259,7 @@
       <c r="B18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="15" t="n">
+      <c r="C18" s="16" t="n">
         <v>308.26</v>
       </c>
       <c r="D18" s="1" t="n">
@@ -1217,7 +1273,7 @@
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="15" t="n">
+      <c r="C19" s="16" t="n">
         <v>340.52</v>
       </c>
       <c r="D19" s="1" t="n">
@@ -1231,7 +1287,7 @@
       <c r="B20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="15" t="n">
+      <c r="C20" s="16" t="n">
         <v>437.01</v>
       </c>
       <c r="D20" s="1" t="n">
@@ -1245,7 +1301,7 @@
       <c r="B21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15" t="n">
+      <c r="C21" s="16" t="n">
         <v>417.24</v>
       </c>
       <c r="D21" s="1" t="n">
@@ -1259,11 +1315,25 @@
       <c r="B22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="16" t="n">
         <v>581.75</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>420</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>612</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added three more cities T and geopotential
</commit_message>
<xml_diff>
--- a/regresiones_era5_observados_conalturas/sesgos_tmax_tmin.xlsx
+++ b/regresiones_era5_observados_conalturas/sesgos_tmax_tmin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t xml:space="preserve">Tmin</t>
   </si>
@@ -245,6 +245,18 @@
     <t xml:space="preserve">Foronda-Txokiza</t>
   </si>
   <si>
+    <t xml:space="preserve">Gasteiz Aeropuerto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebro zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pamplona Aeropuerto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadreita</t>
+  </si>
+  <si>
     <t xml:space="preserve">ERA5Land height</t>
   </si>
   <si>
@@ -260,7 +272,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -326,8 +338,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,11 +373,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6B26B"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFFFF099"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -381,6 +405,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -407,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -428,8 +459,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -440,6 +475,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,6 +492,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -464,11 +507,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,9 +619,9 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFF099"/>
       <rgbColor rgb="FFA4C2F4"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFF6B26B"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFF6B26B"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -553,10 +648,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -619,7 +714,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
@@ -650,7 +745,7 @@
       <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="3" t="s">
@@ -670,680 +765,933 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="9" t="n">
         <v>16.97</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="11" t="n">
         <v>29.12</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G4" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="8" t="n">
         <v>15.35</v>
       </c>
-      <c r="I4" s="11" t="n">
+      <c r="I4" s="13" t="n">
         <f aca="false">D4-H4</f>
         <v>1.62</v>
       </c>
-      <c r="J4" s="8" t="n">
+      <c r="J4" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="11" t="n">
         <v>27.51</v>
       </c>
-      <c r="L4" s="11" t="n">
+      <c r="L4" s="13" t="n">
         <f aca="false">F4-K4</f>
         <v>1.61</v>
       </c>
-      <c r="M4" s="10" t="n">
+      <c r="M4" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="N4" s="7" t="n">
+      <c r="N4" s="8" t="n">
         <v>15.04</v>
       </c>
-      <c r="O4" s="11" t="n">
+      <c r="O4" s="13" t="n">
         <f aca="false">D4-N4</f>
         <v>1.93</v>
       </c>
-      <c r="P4" s="8" t="n">
+      <c r="P4" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="Q4" s="11" t="n">
         <v>27.14</v>
       </c>
-      <c r="R4" s="12" t="n">
+      <c r="R4" s="15" t="n">
         <f aca="false">F4-Q4</f>
         <v>1.98</v>
       </c>
-      <c r="S4" s="6"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="9" t="n">
         <v>15.68</v>
       </c>
-      <c r="E5" s="8" t="n">
+      <c r="E5" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="11" t="n">
         <v>27.05</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="8" t="n">
         <v>15.66</v>
       </c>
-      <c r="I5" s="11" t="n">
+      <c r="I5" s="13" t="n">
         <f aca="false">D5-H5</f>
         <v>0.0199999999999996</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="J5" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="11" t="n">
         <v>27.03</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="13" t="n">
         <f aca="false">F5-K5</f>
         <v>0.0199999999999996</v>
       </c>
-      <c r="M5" s="10" t="n">
+      <c r="M5" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="N5" s="7" t="n">
+      <c r="N5" s="8" t="n">
         <v>13.38</v>
       </c>
-      <c r="O5" s="11" t="n">
+      <c r="O5" s="13" t="n">
         <f aca="false">D5-N5</f>
         <v>2.3</v>
       </c>
-      <c r="P5" s="8" t="n">
+      <c r="P5" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="Q5" s="9" t="n">
+      <c r="Q5" s="11" t="n">
         <v>24.52</v>
       </c>
-      <c r="R5" s="12" t="n">
+      <c r="R5" s="15" t="n">
         <f aca="false">F5-Q5</f>
         <v>2.53</v>
       </c>
-      <c r="S5" s="6"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="9" t="n">
         <v>16.77</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="11" t="n">
         <v>29.37</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="8" t="n">
         <v>16.71</v>
       </c>
-      <c r="I6" s="11" t="n">
+      <c r="I6" s="13" t="n">
         <f aca="false">D6-H6</f>
         <v>0.0599999999999987</v>
       </c>
-      <c r="J6" s="8" t="n">
+      <c r="J6" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="11" t="n">
         <v>29.31</v>
       </c>
-      <c r="L6" s="11" t="n">
+      <c r="L6" s="13" t="n">
         <f aca="false">F6-K6</f>
         <v>0.0600000000000023</v>
       </c>
-      <c r="M6" s="10" t="n">
+      <c r="M6" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="N6" s="7" t="n">
+      <c r="N6" s="8" t="n">
         <v>15.06</v>
       </c>
-      <c r="O6" s="11" t="n">
+      <c r="O6" s="13" t="n">
         <f aca="false">D6-N6</f>
         <v>1.71</v>
       </c>
-      <c r="P6" s="8" t="n">
+      <c r="P6" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="Q6" s="9" t="n">
+      <c r="Q6" s="11" t="n">
         <v>27.55</v>
       </c>
-      <c r="R6" s="12" t="n">
+      <c r="R6" s="15" t="n">
         <f aca="false">F6-Q6</f>
         <v>1.82</v>
       </c>
-      <c r="S6" s="13"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="9" t="n">
         <v>16.93</v>
       </c>
-      <c r="E7" s="8" t="n">
+      <c r="E7" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="11" t="n">
         <v>28.51</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="8" t="n">
         <v>16.76</v>
       </c>
-      <c r="I7" s="11" t="n">
+      <c r="I7" s="13" t="n">
         <f aca="false">D7-H7</f>
         <v>0.169999999999998</v>
       </c>
-      <c r="J7" s="8" t="n">
+      <c r="J7" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="11" t="n">
         <v>28.34</v>
       </c>
-      <c r="L7" s="11" t="n">
+      <c r="L7" s="13" t="n">
         <f aca="false">F7-K7</f>
         <v>0.170000000000002</v>
       </c>
-      <c r="M7" s="10" t="n">
+      <c r="M7" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="N7" s="7" t="n">
+      <c r="N7" s="8" t="n">
         <v>15.29</v>
       </c>
-      <c r="O7" s="11" t="n">
+      <c r="O7" s="13" t="n">
         <f aca="false">D7-N7</f>
         <v>1.64</v>
       </c>
-      <c r="P7" s="8" t="n">
+      <c r="P7" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="Q7" s="9" t="n">
+      <c r="Q7" s="11" t="n">
         <v>26.7</v>
       </c>
-      <c r="R7" s="12" t="n">
+      <c r="R7" s="15" t="n">
         <f aca="false">F7-Q7</f>
         <v>1.81</v>
       </c>
-      <c r="S7" s="13"/>
+      <c r="S7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18" t="n">
+        <f aca="false">SUM(D4:D7)/4</f>
+        <v>16.5875</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20" t="n">
+        <f aca="false">SUM(F7,F6,F5,F4)/4</f>
+        <v>28.5125</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="18" t="n">
+        <f aca="false">SUM(H7,H6,H5,H4)/4</f>
+        <v>16.12</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20" t="n">
+        <f aca="false">SUM(K7,K6,K5,K4)/4</f>
+        <v>28.0475</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C10" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D10" s="9" t="n">
         <v>16.63</v>
       </c>
-      <c r="E8" s="8" t="n">
+      <c r="E10" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F10" s="11" t="n">
         <v>28.56</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G10" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="H10" s="8" t="n">
         <v>16.37</v>
       </c>
-      <c r="I8" s="11" t="n">
-        <f aca="false">D8-H8</f>
+      <c r="I10" s="13" t="n">
+        <f aca="false">D10-H10</f>
         <v>0.259999999999998</v>
       </c>
-      <c r="J8" s="8" t="n">
+      <c r="J10" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K10" s="11" t="n">
         <v>28.3</v>
       </c>
-      <c r="L8" s="11" t="n">
-        <f aca="false">F8-K8</f>
+      <c r="L10" s="13" t="n">
+        <f aca="false">F10-K10</f>
         <v>0.259999999999998</v>
       </c>
-      <c r="M8" s="10" t="n">
+      <c r="M10" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="N8" s="7" t="n">
+      <c r="N10" s="8" t="n">
         <v>15.35</v>
       </c>
-      <c r="O8" s="11" t="n">
-        <f aca="false">D8-N8</f>
+      <c r="O10" s="13" t="n">
+        <f aca="false">D10-N10</f>
         <v>1.28</v>
       </c>
-      <c r="P8" s="8" t="n">
+      <c r="P10" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="Q8" s="9" t="n">
+      <c r="Q10" s="11" t="n">
         <v>27.32</v>
       </c>
-      <c r="R8" s="12" t="n">
-        <f aca="false">F8-Q8</f>
+      <c r="R10" s="15" t="n">
+        <f aca="false">F10-Q10</f>
         <v>1.24</v>
       </c>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C11" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D11" s="9" t="n">
         <v>16.13</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E11" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F11" s="11" t="n">
         <v>32.12</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G11" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H11" s="8" t="n">
         <v>14.8</v>
       </c>
-      <c r="I9" s="11" t="n">
-        <f aca="false">D9-H9</f>
+      <c r="I11" s="13" t="n">
+        <f aca="false">D11-H11</f>
         <v>1.33</v>
       </c>
-      <c r="J9" s="8" t="n">
+      <c r="J11" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K11" s="11" t="n">
         <v>30.78</v>
       </c>
-      <c r="L9" s="11" t="n">
-        <f aca="false">F9-K9</f>
+      <c r="L11" s="13" t="n">
+        <f aca="false">F11-K11</f>
         <v>1.34</v>
       </c>
-      <c r="M9" s="10" t="n">
+      <c r="M11" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="N9" s="7" t="n">
+      <c r="N11" s="8" t="n">
         <v>12.83</v>
       </c>
-      <c r="O9" s="11" t="n">
-        <f aca="false">D9-N9</f>
+      <c r="O11" s="13" t="n">
+        <f aca="false">D11-N11</f>
         <v>3.3</v>
       </c>
-      <c r="P9" s="8" t="n">
+      <c r="P11" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="Q9" s="9" t="n">
+      <c r="Q11" s="11" t="n">
         <v>28.97</v>
       </c>
-      <c r="R9" s="12" t="n">
-        <f aca="false">F9-Q9</f>
+      <c r="R11" s="15" t="n">
+        <f aca="false">F11-Q11</f>
         <v>3.15</v>
       </c>
-      <c r="S9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="S11" s="16"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C12" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D12" s="9" t="n">
         <v>15.75</v>
       </c>
-      <c r="E10" s="8" t="n">
+      <c r="E12" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F12" s="11" t="n">
         <v>33.84</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="G12" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H12" s="8" t="n">
         <v>14.99</v>
       </c>
-      <c r="I10" s="11" t="n">
-        <f aca="false">D10-H10</f>
+      <c r="I12" s="13" t="n">
+        <f aca="false">D12-H12</f>
         <v>0.76</v>
       </c>
-      <c r="J10" s="8" t="n">
+      <c r="J12" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K12" s="11" t="n">
         <v>33.08</v>
       </c>
-      <c r="L10" s="11" t="n">
-        <f aca="false">F10-K10</f>
+      <c r="L12" s="13" t="n">
+        <f aca="false">F12-K12</f>
         <v>0.760000000000005</v>
       </c>
-      <c r="M10" s="10" t="n">
+      <c r="M12" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="N10" s="7" t="n">
+      <c r="N12" s="8" t="n">
         <v>11.93</v>
       </c>
-      <c r="O10" s="11" t="n">
-        <f aca="false">D10-N10</f>
+      <c r="O12" s="13" t="n">
+        <f aca="false">D12-N12</f>
         <v>3.82</v>
       </c>
-      <c r="P10" s="8" t="n">
+      <c r="P12" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="Q10" s="9" t="n">
+      <c r="Q12" s="11" t="n">
         <v>29.87</v>
       </c>
-      <c r="R10" s="12" t="n">
-        <f aca="false">F10-Q10</f>
+      <c r="R12" s="15" t="n">
+        <f aca="false">F12-Q12</f>
         <v>3.97</v>
       </c>
-      <c r="S10" s="13"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C13" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D13" s="9" t="n">
         <v>17.21</v>
       </c>
-      <c r="E11" s="8" t="n">
+      <c r="E13" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F13" s="11" t="n">
         <v>32.87</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G13" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H13" s="8" t="n">
         <v>14.49</v>
       </c>
-      <c r="I11" s="11" t="n">
-        <f aca="false">D11-H11</f>
+      <c r="I13" s="13" t="n">
+        <f aca="false">D13-H13</f>
         <v>2.72</v>
       </c>
-      <c r="J11" s="8" t="n">
+      <c r="J13" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K13" s="11" t="n">
         <v>30.15</v>
       </c>
-      <c r="L11" s="11" t="n">
-        <f aca="false">F11-K11</f>
+      <c r="L13" s="13" t="n">
+        <f aca="false">F13-K13</f>
         <v>2.72</v>
       </c>
-      <c r="M11" s="10" t="n">
+      <c r="M13" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="N11" s="7" t="n">
+      <c r="N13" s="8" t="n">
         <v>13.41</v>
       </c>
-      <c r="O11" s="11" t="n">
-        <f aca="false">D11-N11</f>
+      <c r="O13" s="13" t="n">
+        <f aca="false">D13-N13</f>
         <v>3.8</v>
       </c>
-      <c r="P11" s="8" t="n">
+      <c r="P13" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="Q11" s="9" t="n">
+      <c r="Q13" s="11" t="n">
         <v>29.35</v>
       </c>
-      <c r="R11" s="12" t="n">
-        <f aca="false">F11-Q11</f>
+      <c r="R13" s="15" t="n">
+        <f aca="false">F13-Q13</f>
         <v>3.52</v>
       </c>
-      <c r="S11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
+      <c r="S13" s="16"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18" t="n">
+        <f aca="false">SUM(D10:D13)/4</f>
+        <v>16.43</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20" t="n">
+        <f aca="false">SUM(F13,F12,F11,F10)/4</f>
+        <v>31.8475</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="18" t="n">
+        <f aca="false">SUM(H13,H12,H11,H10)/4</f>
+        <v>15.1625</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20" t="n">
+        <f aca="false">SUM(K13,K12,K11,K10)/4</f>
+        <v>30.5775</v>
+      </c>
+      <c r="L14" s="22"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="16"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="16"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C16" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D16" s="9" t="n">
         <v>16.99</v>
       </c>
-      <c r="E12" s="8" t="n">
+      <c r="E16" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F16" s="11" t="n">
         <v>31.21</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G16" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H16" s="8" t="n">
         <v>16.82</v>
       </c>
-      <c r="I12" s="11" t="n">
-        <f aca="false">D12-H12</f>
+      <c r="I16" s="13" t="n">
+        <f aca="false">D16-H16</f>
         <v>0.169999999999998</v>
       </c>
-      <c r="J12" s="8" t="n">
+      <c r="J16" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K16" s="11" t="n">
         <v>31.04</v>
       </c>
-      <c r="L12" s="11" t="n">
-        <f aca="false">F12-K12</f>
+      <c r="L16" s="13" t="n">
+        <f aca="false">F16-K16</f>
         <v>0.170000000000002</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="3" t="s">
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0"/>
+      <c r="D18" s="18" t="n">
+        <f aca="false">SUM(D16:D17)/2</f>
+        <v>8.495</v>
+      </c>
+      <c r="F18" s="20" t="n">
+        <f aca="false">SUM(F16:F17)/2</f>
+        <v>15.605</v>
+      </c>
+      <c r="H18" s="18" t="n">
+        <f aca="false">SUM(H16:H17)/2</f>
+        <v>8.41</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="20" t="n">
+        <f aca="false">SUM(K16:K17)/2</f>
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="B20" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="16" t="n">
-        <v>361.32</v>
-      </c>
-      <c r="D15" s="1" t="n">
+      <c r="C25" s="32" t="n">
+        <v>123</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="16" t="n">
-        <v>441.31</v>
-      </c>
-      <c r="D16" s="1" t="n">
+      <c r="C26" s="32" t="n">
+        <v>177</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="16" t="n">
-        <v>344.83</v>
-      </c>
-      <c r="D17" s="1" t="n">
+      <c r="C27" s="32" t="n">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B28" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="16" t="n">
-        <v>308.26</v>
-      </c>
-      <c r="D18" s="1" t="n">
+      <c r="C28" s="32" t="n">
+        <v>167</v>
+      </c>
+      <c r="D28" s="1" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="16" t="n">
-        <v>340.52</v>
-      </c>
-      <c r="D19" s="1" t="n">
+      <c r="C29" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="D29" s="1" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="16" t="n">
+      <c r="C30" s="32" t="n">
         <v>437.01</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D30" s="1" t="n">
         <v>208</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B31" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="16" t="n">
-        <v>417.24</v>
-      </c>
-      <c r="D21" s="1" t="n">
+      <c r="C31" s="32" t="n">
+        <v>358</v>
+      </c>
+      <c r="D31" s="1" t="n">
         <v>119</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B32" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="16" t="n">
-        <v>581.75</v>
-      </c>
-      <c r="D22" s="1" t="n">
+      <c r="C32" s="32" t="n">
+        <v>449</v>
+      </c>
+      <c r="D32" s="1" t="n">
         <v>420</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C33" s="1" t="n">
         <v>612</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D33" s="1" t="n">
         <v>513</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>612</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>555</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="30"/>
+      <c r="B36" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:R2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>